<commit_message>
Data cleaning changelog file included.
</commit_message>
<xml_diff>
--- a/Data xlsx/constructors.xlsx
+++ b/Data xlsx/constructors.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analysis\Formula 1\Data xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E60F28E-6593-480F-93B9-4D96A8445FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D8DEF8-2F8C-450F-8AFF-8AAEE0319FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="constructors" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="constructors" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="2" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="629">
   <si>
     <t>constructorId</t>
   </si>
@@ -1895,6 +1899,18 @@
   </si>
   <si>
     <t>http://en.wikipedia.org/wiki/Alpine_F1_Team</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Count of name</t>
   </si>
 </sst>
 </file>
@@ -2378,8 +2394,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2425,7 +2446,43 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2436,6 +2493,1762 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Filipe Silva" refreshedDate="45092.825679513888" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="212" xr:uid="{0B120631-AEF8-41C3-BA76-4A654BBA392F}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C1:C1048576" sheet="constructors"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="name" numFmtId="0">
+      <sharedItems containsBlank="1" count="212">
+        <s v="McLaren"/>
+        <s v="BMW Sauber"/>
+        <s v="Williams"/>
+        <s v="Renault"/>
+        <s v="Toro Rosso"/>
+        <s v="Ferrari"/>
+        <s v="Toyota"/>
+        <s v="Super Aguri"/>
+        <s v="Red Bull"/>
+        <s v="Force India"/>
+        <s v="Honda"/>
+        <s v="Spyker"/>
+        <s v="MF1"/>
+        <s v="Spyker MF1"/>
+        <s v="Sauber"/>
+        <s v="BAR"/>
+        <s v="Jordan"/>
+        <s v="Minardi"/>
+        <s v="Jaguar"/>
+        <s v="Prost"/>
+        <s v="Arrows"/>
+        <s v="Benetton"/>
+        <s v="Brawn"/>
+        <s v="Stewart"/>
+        <s v="Tyrrell"/>
+        <s v="Lola"/>
+        <s v="Ligier"/>
+        <s v="Forti"/>
+        <s v="Footwork"/>
+        <s v="Pacific"/>
+        <s v="Simtek"/>
+        <s v="Team Lotus"/>
+        <s v="Larrousse"/>
+        <s v="Brabham"/>
+        <s v="Dallara"/>
+        <s v="Fondmetal"/>
+        <s v="March"/>
+        <s v="Andrea Moda"/>
+        <s v="AGS"/>
+        <s v="Lambo"/>
+        <s v="Leyton House"/>
+        <s v="Coloni"/>
+        <s v="Euro Brun"/>
+        <s v="Osella"/>
+        <s v="Onyx"/>
+        <s v="Life"/>
+        <s v="Rial"/>
+        <s v="Zakspeed"/>
+        <s v="RAM"/>
+        <s v="Alfa Romeo"/>
+        <s v="Spirit"/>
+        <s v="Toleman"/>
+        <s v="ATS"/>
+        <s v="Theodore"/>
+        <s v="Fittipaldi"/>
+        <s v="Ensign"/>
+        <s v="Shadow"/>
+        <s v="Wolf"/>
+        <s v="Merzario"/>
+        <s v="Kauhsen"/>
+        <s v="Rebaque"/>
+        <s v="Surtees"/>
+        <s v="Hesketh"/>
+        <s v="Martini"/>
+        <s v="BRM"/>
+        <s v="Penske"/>
+        <s v="LEC"/>
+        <s v="McGuire"/>
+        <s v="Boro"/>
+        <s v="Apollon"/>
+        <s v="Kojima"/>
+        <s v="Parnelli"/>
+        <s v="Maki"/>
+        <s v="Embassy Hill"/>
+        <s v="Lyncar"/>
+        <s v="Trojan"/>
+        <s v="Amon"/>
+        <s v="Token"/>
+        <s v="Iso Marlboro"/>
+        <s v="Tecno"/>
+        <s v="Matra"/>
+        <s v="Politoys"/>
+        <s v="Connew"/>
+        <s v="Bellasi"/>
+        <s v="De Tomaso"/>
+        <s v="Cooper"/>
+        <s v="Eagle"/>
+        <s v="LDS"/>
+        <s v="Protos"/>
+        <s v="Shannon"/>
+        <s v="Scirocco"/>
+        <s v="RE"/>
+        <s v="BRP"/>
+        <s v="Porsche"/>
+        <s v="Derrington"/>
+        <s v="Gilby"/>
+        <s v="Stebro"/>
+        <s v="Emeryson"/>
+        <s v="ENB"/>
+        <s v="JBW"/>
+        <s v="Ferguson"/>
+        <s v="MBM"/>
+        <s v="Behra-Porsche"/>
+        <s v="Maserati"/>
+        <s v="Scarab"/>
+        <s v="Watson"/>
+        <s v="Epperly"/>
+        <s v="Phillips"/>
+        <s v="Lesovsky"/>
+        <s v="Trevis"/>
+        <s v="Meskowski"/>
+        <s v="Kurtis Kraft"/>
+        <s v="Kuzma"/>
+        <s v="Christensen"/>
+        <s v="Ewing"/>
+        <s v="Aston Martin"/>
+        <s v="Vanwall"/>
+        <s v="Moore"/>
+        <s v="Dunn"/>
+        <s v="Elder"/>
+        <s v="Sutton"/>
+        <s v="Fry"/>
+        <s v="Tec-Mec"/>
+        <s v="Connaught"/>
+        <s v="Alta"/>
+        <s v="OSCA"/>
+        <s v="Gordini"/>
+        <s v="Stevens"/>
+        <s v="Bugatti"/>
+        <s v="Mercedes"/>
+        <s v="Lancia"/>
+        <s v="HWM"/>
+        <s v="Schroeder"/>
+        <s v="Pawl"/>
+        <s v="Pankratz"/>
+        <s v="Arzani-Volpini"/>
+        <s v="Nichels"/>
+        <s v="Bromme"/>
+        <s v="Klenk"/>
+        <s v="Simca"/>
+        <s v="Turner"/>
+        <s v="Del Roy"/>
+        <s v="Veritas"/>
+        <s v="BMW"/>
+        <s v="EMW"/>
+        <s v="AFM"/>
+        <s v="Frazer Nash"/>
+        <s v="Sherman"/>
+        <s v="Deidt"/>
+        <s v="ERA"/>
+        <s v="Aston Butterworth"/>
+        <s v="Cisitalia"/>
+        <s v="Talbot-Lago"/>
+        <s v="Hall"/>
+        <s v="Marchese"/>
+        <s v="Langley"/>
+        <s v="Rae"/>
+        <s v="Olson"/>
+        <s v="Wetteroth"/>
+        <s v="Adams"/>
+        <s v="Snowberger"/>
+        <s v="Milano"/>
+        <s v="HRT"/>
+        <s v="Cooper-Maserati"/>
+        <s v="Virgin"/>
+        <s v="Cooper-OSCA"/>
+        <s v="Cooper-Borgward"/>
+        <s v="Cooper-Climax"/>
+        <s v="Cooper-Castellotti"/>
+        <s v="Lotus-Climax"/>
+        <s v="Lotus-Maserati"/>
+        <s v="De Tomaso-Osca"/>
+        <s v="De Tomaso-Alfa Romeo"/>
+        <s v="Lotus-BRM"/>
+        <s v="Lotus-Borgward"/>
+        <s v="Cooper-Alfa Romeo"/>
+        <s v="De Tomaso-Ferrari"/>
+        <s v="Lotus-Ford"/>
+        <s v="Brabham-BRM"/>
+        <s v="Brabham-Ford"/>
+        <s v="Brabham-Climax"/>
+        <s v="LDS-Climax"/>
+        <s v="LDS-Alfa Romeo"/>
+        <s v="Cooper-Ford"/>
+        <s v="McLaren-Ford"/>
+        <s v="McLaren-Serenissima"/>
+        <s v="Eagle-Climax"/>
+        <s v="Eagle-Weslake"/>
+        <s v="Brabham-Repco"/>
+        <s v="Cooper-Ferrari"/>
+        <s v="Cooper-ATS"/>
+        <s v="McLaren-BRM"/>
+        <s v="Cooper-BRM"/>
+        <s v="Matra-Ford"/>
+        <s v="BRM-Ford"/>
+        <s v="McLaren-Alfa Romeo"/>
+        <s v="March-Alfa Romeo"/>
+        <s v="March-Ford"/>
+        <s v="Lotus-Pratt &amp;amp; Whitney"/>
+        <s v="Shadow-Ford"/>
+        <s v="Shadow-Matra"/>
+        <s v="Brabham-Alfa Romeo"/>
+        <s v="Lotus"/>
+        <s v="Marussia"/>
+        <s v="Caterham"/>
+        <s v="Lotus F1"/>
+        <s v="Manor Marussia"/>
+        <s v="Haas F1 Team"/>
+        <s v="Racing Point"/>
+        <s v="AlphaTauri"/>
+        <s v="Alpine F1 Team"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="212">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="34"/>
+  </r>
+  <r>
+    <x v="35"/>
+  </r>
+  <r>
+    <x v="36"/>
+  </r>
+  <r>
+    <x v="37"/>
+  </r>
+  <r>
+    <x v="38"/>
+  </r>
+  <r>
+    <x v="39"/>
+  </r>
+  <r>
+    <x v="40"/>
+  </r>
+  <r>
+    <x v="41"/>
+  </r>
+  <r>
+    <x v="42"/>
+  </r>
+  <r>
+    <x v="43"/>
+  </r>
+  <r>
+    <x v="44"/>
+  </r>
+  <r>
+    <x v="45"/>
+  </r>
+  <r>
+    <x v="46"/>
+  </r>
+  <r>
+    <x v="47"/>
+  </r>
+  <r>
+    <x v="48"/>
+  </r>
+  <r>
+    <x v="49"/>
+  </r>
+  <r>
+    <x v="50"/>
+  </r>
+  <r>
+    <x v="51"/>
+  </r>
+  <r>
+    <x v="52"/>
+  </r>
+  <r>
+    <x v="53"/>
+  </r>
+  <r>
+    <x v="54"/>
+  </r>
+  <r>
+    <x v="55"/>
+  </r>
+  <r>
+    <x v="56"/>
+  </r>
+  <r>
+    <x v="57"/>
+  </r>
+  <r>
+    <x v="58"/>
+  </r>
+  <r>
+    <x v="59"/>
+  </r>
+  <r>
+    <x v="60"/>
+  </r>
+  <r>
+    <x v="61"/>
+  </r>
+  <r>
+    <x v="62"/>
+  </r>
+  <r>
+    <x v="63"/>
+  </r>
+  <r>
+    <x v="64"/>
+  </r>
+  <r>
+    <x v="65"/>
+  </r>
+  <r>
+    <x v="66"/>
+  </r>
+  <r>
+    <x v="67"/>
+  </r>
+  <r>
+    <x v="68"/>
+  </r>
+  <r>
+    <x v="69"/>
+  </r>
+  <r>
+    <x v="70"/>
+  </r>
+  <r>
+    <x v="71"/>
+  </r>
+  <r>
+    <x v="72"/>
+  </r>
+  <r>
+    <x v="73"/>
+  </r>
+  <r>
+    <x v="74"/>
+  </r>
+  <r>
+    <x v="75"/>
+  </r>
+  <r>
+    <x v="76"/>
+  </r>
+  <r>
+    <x v="77"/>
+  </r>
+  <r>
+    <x v="78"/>
+  </r>
+  <r>
+    <x v="79"/>
+  </r>
+  <r>
+    <x v="80"/>
+  </r>
+  <r>
+    <x v="81"/>
+  </r>
+  <r>
+    <x v="82"/>
+  </r>
+  <r>
+    <x v="83"/>
+  </r>
+  <r>
+    <x v="84"/>
+  </r>
+  <r>
+    <x v="85"/>
+  </r>
+  <r>
+    <x v="86"/>
+  </r>
+  <r>
+    <x v="87"/>
+  </r>
+  <r>
+    <x v="88"/>
+  </r>
+  <r>
+    <x v="89"/>
+  </r>
+  <r>
+    <x v="90"/>
+  </r>
+  <r>
+    <x v="91"/>
+  </r>
+  <r>
+    <x v="92"/>
+  </r>
+  <r>
+    <x v="93"/>
+  </r>
+  <r>
+    <x v="94"/>
+  </r>
+  <r>
+    <x v="95"/>
+  </r>
+  <r>
+    <x v="96"/>
+  </r>
+  <r>
+    <x v="97"/>
+  </r>
+  <r>
+    <x v="98"/>
+  </r>
+  <r>
+    <x v="99"/>
+  </r>
+  <r>
+    <x v="100"/>
+  </r>
+  <r>
+    <x v="101"/>
+  </r>
+  <r>
+    <x v="102"/>
+  </r>
+  <r>
+    <x v="103"/>
+  </r>
+  <r>
+    <x v="104"/>
+  </r>
+  <r>
+    <x v="105"/>
+  </r>
+  <r>
+    <x v="106"/>
+  </r>
+  <r>
+    <x v="107"/>
+  </r>
+  <r>
+    <x v="108"/>
+  </r>
+  <r>
+    <x v="109"/>
+  </r>
+  <r>
+    <x v="110"/>
+  </r>
+  <r>
+    <x v="111"/>
+  </r>
+  <r>
+    <x v="112"/>
+  </r>
+  <r>
+    <x v="113"/>
+  </r>
+  <r>
+    <x v="114"/>
+  </r>
+  <r>
+    <x v="115"/>
+  </r>
+  <r>
+    <x v="116"/>
+  </r>
+  <r>
+    <x v="117"/>
+  </r>
+  <r>
+    <x v="118"/>
+  </r>
+  <r>
+    <x v="119"/>
+  </r>
+  <r>
+    <x v="120"/>
+  </r>
+  <r>
+    <x v="121"/>
+  </r>
+  <r>
+    <x v="122"/>
+  </r>
+  <r>
+    <x v="123"/>
+  </r>
+  <r>
+    <x v="124"/>
+  </r>
+  <r>
+    <x v="125"/>
+  </r>
+  <r>
+    <x v="126"/>
+  </r>
+  <r>
+    <x v="127"/>
+  </r>
+  <r>
+    <x v="128"/>
+  </r>
+  <r>
+    <x v="129"/>
+  </r>
+  <r>
+    <x v="130"/>
+  </r>
+  <r>
+    <x v="131"/>
+  </r>
+  <r>
+    <x v="132"/>
+  </r>
+  <r>
+    <x v="133"/>
+  </r>
+  <r>
+    <x v="134"/>
+  </r>
+  <r>
+    <x v="135"/>
+  </r>
+  <r>
+    <x v="136"/>
+  </r>
+  <r>
+    <x v="137"/>
+  </r>
+  <r>
+    <x v="138"/>
+  </r>
+  <r>
+    <x v="139"/>
+  </r>
+  <r>
+    <x v="140"/>
+  </r>
+  <r>
+    <x v="141"/>
+  </r>
+  <r>
+    <x v="142"/>
+  </r>
+  <r>
+    <x v="143"/>
+  </r>
+  <r>
+    <x v="144"/>
+  </r>
+  <r>
+    <x v="145"/>
+  </r>
+  <r>
+    <x v="146"/>
+  </r>
+  <r>
+    <x v="147"/>
+  </r>
+  <r>
+    <x v="148"/>
+  </r>
+  <r>
+    <x v="149"/>
+  </r>
+  <r>
+    <x v="150"/>
+  </r>
+  <r>
+    <x v="151"/>
+  </r>
+  <r>
+    <x v="152"/>
+  </r>
+  <r>
+    <x v="153"/>
+  </r>
+  <r>
+    <x v="154"/>
+  </r>
+  <r>
+    <x v="155"/>
+  </r>
+  <r>
+    <x v="156"/>
+  </r>
+  <r>
+    <x v="157"/>
+  </r>
+  <r>
+    <x v="158"/>
+  </r>
+  <r>
+    <x v="159"/>
+  </r>
+  <r>
+    <x v="160"/>
+  </r>
+  <r>
+    <x v="161"/>
+  </r>
+  <r>
+    <x v="162"/>
+  </r>
+  <r>
+    <x v="163"/>
+  </r>
+  <r>
+    <x v="164"/>
+  </r>
+  <r>
+    <x v="165"/>
+  </r>
+  <r>
+    <x v="166"/>
+  </r>
+  <r>
+    <x v="167"/>
+  </r>
+  <r>
+    <x v="168"/>
+  </r>
+  <r>
+    <x v="169"/>
+  </r>
+  <r>
+    <x v="170"/>
+  </r>
+  <r>
+    <x v="171"/>
+  </r>
+  <r>
+    <x v="172"/>
+  </r>
+  <r>
+    <x v="173"/>
+  </r>
+  <r>
+    <x v="174"/>
+  </r>
+  <r>
+    <x v="175"/>
+  </r>
+  <r>
+    <x v="176"/>
+  </r>
+  <r>
+    <x v="177"/>
+  </r>
+  <r>
+    <x v="178"/>
+  </r>
+  <r>
+    <x v="179"/>
+  </r>
+  <r>
+    <x v="180"/>
+  </r>
+  <r>
+    <x v="181"/>
+  </r>
+  <r>
+    <x v="182"/>
+  </r>
+  <r>
+    <x v="183"/>
+  </r>
+  <r>
+    <x v="184"/>
+  </r>
+  <r>
+    <x v="185"/>
+  </r>
+  <r>
+    <x v="186"/>
+  </r>
+  <r>
+    <x v="187"/>
+  </r>
+  <r>
+    <x v="188"/>
+  </r>
+  <r>
+    <x v="189"/>
+  </r>
+  <r>
+    <x v="190"/>
+  </r>
+  <r>
+    <x v="191"/>
+  </r>
+  <r>
+    <x v="192"/>
+  </r>
+  <r>
+    <x v="193"/>
+  </r>
+  <r>
+    <x v="194"/>
+  </r>
+  <r>
+    <x v="195"/>
+  </r>
+  <r>
+    <x v="196"/>
+  </r>
+  <r>
+    <x v="197"/>
+  </r>
+  <r>
+    <x v="198"/>
+  </r>
+  <r>
+    <x v="199"/>
+  </r>
+  <r>
+    <x v="200"/>
+  </r>
+  <r>
+    <x v="201"/>
+  </r>
+  <r>
+    <x v="202"/>
+  </r>
+  <r>
+    <x v="203"/>
+  </r>
+  <r>
+    <x v="204"/>
+  </r>
+  <r>
+    <x v="205"/>
+  </r>
+  <r>
+    <x v="206"/>
+  </r>
+  <r>
+    <x v="207"/>
+  </r>
+  <r>
+    <x v="208"/>
+  </r>
+  <r>
+    <x v="209"/>
+  </r>
+  <r>
+    <x v="210"/>
+  </r>
+  <r>
+    <x v="211"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74E316E5-0DFC-4695-9DE8-4B34A47BF3F9}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B216" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="213">
+        <item x="36"/>
+        <item x="159"/>
+        <item x="145"/>
+        <item x="38"/>
+        <item x="49"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="124"/>
+        <item x="76"/>
+        <item x="37"/>
+        <item x="69"/>
+        <item x="20"/>
+        <item x="135"/>
+        <item x="150"/>
+        <item x="115"/>
+        <item x="52"/>
+        <item x="15"/>
+        <item x="102"/>
+        <item x="83"/>
+        <item x="21"/>
+        <item x="143"/>
+        <item x="1"/>
+        <item x="68"/>
+        <item x="33"/>
+        <item x="201"/>
+        <item x="178"/>
+        <item x="180"/>
+        <item x="179"/>
+        <item x="188"/>
+        <item x="22"/>
+        <item x="64"/>
+        <item x="194"/>
+        <item x="137"/>
+        <item x="92"/>
+        <item x="128"/>
+        <item x="204"/>
+        <item x="113"/>
+        <item x="151"/>
+        <item x="41"/>
+        <item x="123"/>
+        <item x="82"/>
+        <item x="85"/>
+        <item x="175"/>
+        <item x="190"/>
+        <item x="166"/>
+        <item x="192"/>
+        <item x="168"/>
+        <item x="167"/>
+        <item x="189"/>
+        <item x="183"/>
+        <item x="163"/>
+        <item x="165"/>
+        <item x="34"/>
+        <item x="84"/>
+        <item x="172"/>
+        <item x="176"/>
+        <item x="171"/>
+        <item x="148"/>
+        <item x="141"/>
+        <item x="94"/>
+        <item x="118"/>
+        <item x="86"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="119"/>
+        <item x="73"/>
+        <item x="97"/>
+        <item x="144"/>
+        <item x="98"/>
+        <item x="55"/>
+        <item x="106"/>
+        <item x="149"/>
+        <item x="42"/>
+        <item x="114"/>
+        <item x="100"/>
+        <item x="5"/>
+        <item x="54"/>
+        <item x="35"/>
+        <item x="28"/>
+        <item x="9"/>
+        <item x="27"/>
+        <item x="146"/>
+        <item x="121"/>
+        <item x="95"/>
+        <item x="126"/>
+        <item x="207"/>
+        <item x="153"/>
+        <item x="62"/>
+        <item x="10"/>
+        <item x="162"/>
+        <item x="131"/>
+        <item x="78"/>
+        <item x="18"/>
+        <item x="99"/>
+        <item x="16"/>
+        <item x="59"/>
+        <item x="138"/>
+        <item x="70"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="39"/>
+        <item x="130"/>
+        <item x="155"/>
+        <item x="32"/>
+        <item x="87"/>
+        <item x="182"/>
+        <item x="181"/>
+        <item x="66"/>
+        <item x="108"/>
+        <item x="40"/>
+        <item x="45"/>
+        <item x="26"/>
+        <item x="25"/>
+        <item x="202"/>
+        <item x="205"/>
+        <item x="174"/>
+        <item x="173"/>
+        <item x="169"/>
+        <item x="177"/>
+        <item x="170"/>
+        <item x="198"/>
+        <item x="74"/>
+        <item x="72"/>
+        <item x="206"/>
+        <item x="196"/>
+        <item x="154"/>
+        <item x="197"/>
+        <item x="63"/>
+        <item x="203"/>
+        <item x="103"/>
+        <item x="80"/>
+        <item x="193"/>
+        <item x="101"/>
+        <item x="67"/>
+        <item x="0"/>
+        <item x="195"/>
+        <item x="191"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="129"/>
+        <item x="58"/>
+        <item x="110"/>
+        <item x="12"/>
+        <item x="161"/>
+        <item x="17"/>
+        <item x="117"/>
+        <item x="136"/>
+        <item x="157"/>
+        <item x="44"/>
+        <item x="125"/>
+        <item x="43"/>
+        <item x="29"/>
+        <item x="134"/>
+        <item x="71"/>
+        <item x="133"/>
+        <item x="65"/>
+        <item x="107"/>
+        <item x="81"/>
+        <item x="93"/>
+        <item x="19"/>
+        <item x="88"/>
+        <item x="208"/>
+        <item x="156"/>
+        <item x="48"/>
+        <item x="91"/>
+        <item x="60"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="46"/>
+        <item x="14"/>
+        <item x="104"/>
+        <item x="132"/>
+        <item x="90"/>
+        <item x="56"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="89"/>
+        <item x="147"/>
+        <item x="139"/>
+        <item x="30"/>
+        <item x="160"/>
+        <item x="50"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="96"/>
+        <item x="127"/>
+        <item x="23"/>
+        <item x="7"/>
+        <item x="61"/>
+        <item x="120"/>
+        <item x="152"/>
+        <item x="31"/>
+        <item x="122"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="109"/>
+        <item x="75"/>
+        <item x="140"/>
+        <item x="24"/>
+        <item x="116"/>
+        <item x="142"/>
+        <item x="164"/>
+        <item x="105"/>
+        <item x="158"/>
+        <item x="2"/>
+        <item x="57"/>
+        <item x="47"/>
+        <item x="211"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="213">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="78"/>
+    </i>
+    <i>
+      <x v="79"/>
+    </i>
+    <i>
+      <x v="80"/>
+    </i>
+    <i>
+      <x v="81"/>
+    </i>
+    <i>
+      <x v="82"/>
+    </i>
+    <i>
+      <x v="83"/>
+    </i>
+    <i>
+      <x v="84"/>
+    </i>
+    <i>
+      <x v="85"/>
+    </i>
+    <i>
+      <x v="86"/>
+    </i>
+    <i>
+      <x v="87"/>
+    </i>
+    <i>
+      <x v="88"/>
+    </i>
+    <i>
+      <x v="89"/>
+    </i>
+    <i>
+      <x v="90"/>
+    </i>
+    <i>
+      <x v="91"/>
+    </i>
+    <i>
+      <x v="92"/>
+    </i>
+    <i>
+      <x v="93"/>
+    </i>
+    <i>
+      <x v="94"/>
+    </i>
+    <i>
+      <x v="95"/>
+    </i>
+    <i>
+      <x v="96"/>
+    </i>
+    <i>
+      <x v="97"/>
+    </i>
+    <i>
+      <x v="98"/>
+    </i>
+    <i>
+      <x v="99"/>
+    </i>
+    <i>
+      <x v="100"/>
+    </i>
+    <i>
+      <x v="101"/>
+    </i>
+    <i>
+      <x v="102"/>
+    </i>
+    <i>
+      <x v="103"/>
+    </i>
+    <i>
+      <x v="104"/>
+    </i>
+    <i>
+      <x v="105"/>
+    </i>
+    <i>
+      <x v="106"/>
+    </i>
+    <i>
+      <x v="107"/>
+    </i>
+    <i>
+      <x v="108"/>
+    </i>
+    <i>
+      <x v="109"/>
+    </i>
+    <i>
+      <x v="110"/>
+    </i>
+    <i>
+      <x v="111"/>
+    </i>
+    <i>
+      <x v="112"/>
+    </i>
+    <i>
+      <x v="113"/>
+    </i>
+    <i>
+      <x v="114"/>
+    </i>
+    <i>
+      <x v="115"/>
+    </i>
+    <i>
+      <x v="116"/>
+    </i>
+    <i>
+      <x v="117"/>
+    </i>
+    <i>
+      <x v="118"/>
+    </i>
+    <i>
+      <x v="119"/>
+    </i>
+    <i>
+      <x v="120"/>
+    </i>
+    <i>
+      <x v="121"/>
+    </i>
+    <i>
+      <x v="122"/>
+    </i>
+    <i>
+      <x v="123"/>
+    </i>
+    <i>
+      <x v="124"/>
+    </i>
+    <i>
+      <x v="125"/>
+    </i>
+    <i>
+      <x v="126"/>
+    </i>
+    <i>
+      <x v="127"/>
+    </i>
+    <i>
+      <x v="128"/>
+    </i>
+    <i>
+      <x v="129"/>
+    </i>
+    <i>
+      <x v="130"/>
+    </i>
+    <i>
+      <x v="131"/>
+    </i>
+    <i>
+      <x v="132"/>
+    </i>
+    <i>
+      <x v="133"/>
+    </i>
+    <i>
+      <x v="134"/>
+    </i>
+    <i>
+      <x v="135"/>
+    </i>
+    <i>
+      <x v="136"/>
+    </i>
+    <i>
+      <x v="137"/>
+    </i>
+    <i>
+      <x v="138"/>
+    </i>
+    <i>
+      <x v="139"/>
+    </i>
+    <i>
+      <x v="140"/>
+    </i>
+    <i>
+      <x v="141"/>
+    </i>
+    <i>
+      <x v="142"/>
+    </i>
+    <i>
+      <x v="143"/>
+    </i>
+    <i>
+      <x v="144"/>
+    </i>
+    <i>
+      <x v="145"/>
+    </i>
+    <i>
+      <x v="146"/>
+    </i>
+    <i>
+      <x v="147"/>
+    </i>
+    <i>
+      <x v="148"/>
+    </i>
+    <i>
+      <x v="149"/>
+    </i>
+    <i>
+      <x v="150"/>
+    </i>
+    <i>
+      <x v="151"/>
+    </i>
+    <i>
+      <x v="152"/>
+    </i>
+    <i>
+      <x v="153"/>
+    </i>
+    <i>
+      <x v="154"/>
+    </i>
+    <i>
+      <x v="155"/>
+    </i>
+    <i>
+      <x v="156"/>
+    </i>
+    <i>
+      <x v="157"/>
+    </i>
+    <i>
+      <x v="158"/>
+    </i>
+    <i>
+      <x v="159"/>
+    </i>
+    <i>
+      <x v="160"/>
+    </i>
+    <i>
+      <x v="161"/>
+    </i>
+    <i>
+      <x v="162"/>
+    </i>
+    <i>
+      <x v="163"/>
+    </i>
+    <i>
+      <x v="164"/>
+    </i>
+    <i>
+      <x v="165"/>
+    </i>
+    <i>
+      <x v="166"/>
+    </i>
+    <i>
+      <x v="167"/>
+    </i>
+    <i>
+      <x v="168"/>
+    </i>
+    <i>
+      <x v="169"/>
+    </i>
+    <i>
+      <x v="170"/>
+    </i>
+    <i>
+      <x v="171"/>
+    </i>
+    <i>
+      <x v="172"/>
+    </i>
+    <i>
+      <x v="173"/>
+    </i>
+    <i>
+      <x v="174"/>
+    </i>
+    <i>
+      <x v="175"/>
+    </i>
+    <i>
+      <x v="176"/>
+    </i>
+    <i>
+      <x v="177"/>
+    </i>
+    <i>
+      <x v="178"/>
+    </i>
+    <i>
+      <x v="179"/>
+    </i>
+    <i>
+      <x v="180"/>
+    </i>
+    <i>
+      <x v="181"/>
+    </i>
+    <i>
+      <x v="182"/>
+    </i>
+    <i>
+      <x v="183"/>
+    </i>
+    <i>
+      <x v="184"/>
+    </i>
+    <i>
+      <x v="185"/>
+    </i>
+    <i>
+      <x v="186"/>
+    </i>
+    <i>
+      <x v="187"/>
+    </i>
+    <i>
+      <x v="188"/>
+    </i>
+    <i>
+      <x v="189"/>
+    </i>
+    <i>
+      <x v="190"/>
+    </i>
+    <i>
+      <x v="191"/>
+    </i>
+    <i>
+      <x v="192"/>
+    </i>
+    <i>
+      <x v="193"/>
+    </i>
+    <i>
+      <x v="194"/>
+    </i>
+    <i>
+      <x v="195"/>
+    </i>
+    <i>
+      <x v="196"/>
+    </i>
+    <i>
+      <x v="197"/>
+    </i>
+    <i>
+      <x v="198"/>
+    </i>
+    <i>
+      <x v="199"/>
+    </i>
+    <i>
+      <x v="200"/>
+    </i>
+    <i>
+      <x v="201"/>
+    </i>
+    <i>
+      <x v="202"/>
+    </i>
+    <i>
+      <x v="203"/>
+    </i>
+    <i>
+      <x v="204"/>
+    </i>
+    <i>
+      <x v="205"/>
+    </i>
+    <i>
+      <x v="206"/>
+    </i>
+    <i>
+      <x v="207"/>
+    </i>
+    <i>
+      <x v="208"/>
+    </i>
+    <i>
+      <x v="209"/>
+    </i>
+    <i>
+      <x v="210"/>
+    </i>
+    <i>
+      <x v="211"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2748,11 +4561,1742 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A9397C-6115-4223-9D5B-F1D30D8E2CCC}">
+  <dimension ref="A3:B216"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="212" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B3" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B90" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B92" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B98" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B104" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B105" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B108" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B109" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B110" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B112" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B113" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B114" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B115" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B117" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B118" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B119" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B120" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B121" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B122" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B123" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B124" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B125" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B126" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="B127" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B128" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B129" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B130" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B131" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B132" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B133" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B134" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B135" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B136" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B137" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B141" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B142" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B143" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B144" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B145" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B146" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B147" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B148" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B149" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B150" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B151" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B152" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B153" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B154" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B155" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B156" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B157" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B158" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B159" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B160" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B161" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B162" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B163" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B164" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B165" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B166" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B167" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B168" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B169" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B170" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B171" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B172" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B173" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B174" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B175" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B176" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B177" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B178" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B179" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B180" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B181" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B182" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B183" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B184" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B185" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B186" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B187" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B188" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B189" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B190" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B191" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B192" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B193" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B194" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B195" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B196" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B197" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B198" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B199" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B200" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B201" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B202" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B203" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B204" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B205" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B206" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B207" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B208" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B209" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B210" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B211" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B212" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B213" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B214" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B215" s="3"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B216" s="3">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6369,9 +9913,15 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:E212">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>